<commit_message>
update example excel sheet
</commit_message>
<xml_diff>
--- a/pyscript/genereratark.xlsx
+++ b/pyscript/genereratark.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="164">
   <si>
     <t>Vecka</t>
   </si>
@@ -34,6 +34,33 @@
     <t>Match ID</t>
   </si>
   <si>
+    <t>Thu, 01 Jan</t>
+  </si>
+  <si>
+    <t>01:00</t>
+  </si>
+  <si>
+    <t>Sydväst Ungdom Grön serie U12 A</t>
+  </si>
+  <si>
+    <t>reby IS P11</t>
+  </si>
+  <si>
+    <t>SK Höjden Flickor</t>
+  </si>
+  <si>
+    <t>30579212</t>
+  </si>
+  <si>
+    <t>K Kungälv</t>
+  </si>
+  <si>
+    <t>Surte BK</t>
+  </si>
+  <si>
+    <t>30579213</t>
+  </si>
+  <si>
     <t>Sat, 03 Nov</t>
   </si>
   <si>
@@ -67,6 +94,18 @@
     <t>Sat, 17 Nov</t>
   </si>
   <si>
+    <t>00:00</t>
+  </si>
+  <si>
+    <t>Sydväst Ungdom Svart serie U14 A</t>
+  </si>
+  <si>
+    <t>Oskarströms BK</t>
+  </si>
+  <si>
+    <t>30579249</t>
+  </si>
+  <si>
     <t>13:00</t>
   </si>
   <si>
@@ -82,12 +121,21 @@
     <t>30537322</t>
   </si>
   <si>
+    <t>Sat, 24 Nov</t>
+  </si>
+  <si>
+    <t>Herr Div 2 Sydväst</t>
+  </si>
+  <si>
+    <t>Kungälvs SK</t>
+  </si>
+  <si>
+    <t>30580244</t>
+  </si>
+  <si>
     <t>Sun, 25 Nov</t>
   </si>
   <si>
-    <t>00:00</t>
-  </si>
-  <si>
     <t>P16 Kakservice Syd</t>
   </si>
   <si>
@@ -103,6 +151,18 @@
     <t>Sat, 01 Dec</t>
   </si>
   <si>
+    <t>Frillesås/Sunvära</t>
+  </si>
+  <si>
+    <t>30579254</t>
+  </si>
+  <si>
+    <t>Kareby IS P11</t>
+  </si>
+  <si>
+    <t>30579181</t>
+  </si>
+  <si>
     <t>16:00</t>
   </si>
   <si>
@@ -136,6 +196,9 @@
     <t>30537409</t>
   </si>
   <si>
+    <t>30579184</t>
+  </si>
+  <si>
     <t>Tranås BoIS</t>
   </si>
   <si>
@@ -151,18 +214,33 @@
     <t>30543346</t>
   </si>
   <si>
+    <t>Ungdom P 14 A Västergötland</t>
+  </si>
+  <si>
+    <t>Villa/LAIK Flick</t>
+  </si>
+  <si>
+    <t>30576081</t>
+  </si>
+  <si>
     <t>Vargöns BK</t>
   </si>
   <si>
     <t>30537340</t>
   </si>
   <si>
+    <t>Sat, 15 Dec</t>
+  </si>
+  <si>
+    <t>Torup</t>
+  </si>
+  <si>
+    <t>30580254</t>
+  </si>
+  <si>
     <t>Wed, 19 Dec</t>
   </si>
   <si>
-    <t>Surte BK</t>
-  </si>
-  <si>
     <t>30537345</t>
   </si>
   <si>
@@ -175,6 +253,12 @@
     <t>30537415</t>
   </si>
   <si>
+    <t>LAIK</t>
+  </si>
+  <si>
+    <t>30576088</t>
+  </si>
+  <si>
     <t>LAIK U</t>
   </si>
   <si>
@@ -184,6 +268,21 @@
     <t>Sat, 29 Dec</t>
   </si>
   <si>
+    <t>Mölndal Bandy</t>
+  </si>
+  <si>
+    <t>30579263</t>
+  </si>
+  <si>
+    <t>SK Höjden</t>
+  </si>
+  <si>
+    <t>30579190</t>
+  </si>
+  <si>
+    <t>30579189</t>
+  </si>
+  <si>
     <t>Gripen Trollhättan BK</t>
   </si>
   <si>
@@ -193,63 +292,99 @@
     <t>Sun, 30 Dec</t>
   </si>
   <si>
+    <t>Nässjö/Målilla</t>
+  </si>
+  <si>
+    <t>30543354</t>
+  </si>
+  <si>
+    <t>Blåsuts BK</t>
+  </si>
+  <si>
+    <t>30537358</t>
+  </si>
+  <si>
+    <t>Sat, 05 Jan</t>
+  </si>
+  <si>
+    <t>30580260</t>
+  </si>
+  <si>
+    <t>Sat, 12 Jan</t>
+  </si>
+  <si>
+    <t>IFK Vänersborg</t>
+  </si>
+  <si>
+    <t>30537420</t>
+  </si>
+  <si>
+    <t>Karlstad Bandy</t>
+  </si>
+  <si>
+    <t>30576091</t>
+  </si>
+  <si>
+    <t>30579194</t>
+  </si>
+  <si>
+    <t>30579195</t>
+  </si>
+  <si>
+    <t>Peace &amp; Love City Bandy</t>
+  </si>
+  <si>
+    <t>30476017</t>
+  </si>
+  <si>
+    <t>Sun, 13 Jan</t>
+  </si>
+  <si>
+    <t>Vänersborg/Blåsut</t>
+  </si>
+  <si>
+    <t>30543365</t>
+  </si>
+  <si>
+    <t>30537365</t>
+  </si>
+  <si>
+    <t>IFK Rättvik</t>
+  </si>
+  <si>
+    <t>30476029</t>
+  </si>
+  <si>
+    <t>Sat, 19 Jan</t>
+  </si>
+  <si>
+    <t>30576092</t>
+  </si>
+  <si>
+    <t>Villa Lidköping BK (04 blå)</t>
+  </si>
+  <si>
+    <t>30579271</t>
+  </si>
+  <si>
+    <t>30579199</t>
+  </si>
+  <si>
+    <t>Sat, 26 Jan</t>
+  </si>
+  <si>
+    <t>Höjden/Mölndal</t>
+  </si>
+  <si>
+    <t>30537428</t>
+  </si>
+  <si>
+    <t>30579202</t>
+  </si>
+  <si>
     <t>Nässjö IF</t>
   </si>
   <si>
-    <t>30543354</t>
-  </si>
-  <si>
-    <t>Blåsuts BK</t>
-  </si>
-  <si>
-    <t>30537358</t>
-  </si>
-  <si>
-    <t>Sat, 12 Jan</t>
-  </si>
-  <si>
-    <t>IFK Vänersborg</t>
-  </si>
-  <si>
-    <t>30537420</t>
-  </si>
-  <si>
-    <t>Peace &amp; Love City Bandy</t>
-  </si>
-  <si>
-    <t>30476017</t>
-  </si>
-  <si>
-    <t>Sun, 13 Jan</t>
-  </si>
-  <si>
-    <t>Vänersborg/Blåsut</t>
-  </si>
-  <si>
-    <t>30543365</t>
-  </si>
-  <si>
-    <t>Mölndal Bandy</t>
-  </si>
-  <si>
-    <t>30537365</t>
-  </si>
-  <si>
-    <t>IFK Rättvik</t>
-  </si>
-  <si>
-    <t>30476029</t>
-  </si>
-  <si>
-    <t>Sat, 26 Jan</t>
-  </si>
-  <si>
-    <t>SK Höjden</t>
-  </si>
-  <si>
-    <t>30537428</t>
-  </si>
-  <si>
     <t>30476052</t>
   </si>
   <si>
@@ -271,18 +406,36 @@
     <t>Sat, 02 Feb</t>
   </si>
   <si>
+    <t>30580270</t>
+  </si>
+  <si>
     <t>30537381</t>
   </si>
   <si>
     <t>Sat, 09 Feb</t>
   </si>
   <si>
-    <t>Karlstad Bandy</t>
-  </si>
-  <si>
     <t>30537433</t>
   </si>
   <si>
+    <t>Villa Lidköping BK (vit)</t>
+  </si>
+  <si>
+    <t>30576099</t>
+  </si>
+  <si>
+    <t>Surte/Kareby</t>
+  </si>
+  <si>
+    <t>30579280</t>
+  </si>
+  <si>
+    <t>30579207</t>
+  </si>
+  <si>
+    <t>30579208</t>
+  </si>
+  <si>
     <t>ÅbyTjureda IF</t>
   </si>
   <si>
@@ -301,12 +454,27 @@
     <t>30537389</t>
   </si>
   <si>
+    <t>Sat, 16 Feb</t>
+  </si>
+  <si>
+    <t>Vildkatterna</t>
+  </si>
+  <si>
+    <t>30580276</t>
+  </si>
+  <si>
     <t>Sat, 23 Feb</t>
   </si>
   <si>
     <t>30537438</t>
   </si>
   <si>
+    <t>BK Slottshov</t>
+  </si>
+  <si>
+    <t>30580280</t>
+  </si>
+  <si>
     <t>Örebro SK</t>
   </si>
   <si>
@@ -323,6 +491,12 @@
   </si>
   <si>
     <t>30537396</t>
+  </si>
+  <si>
+    <t>Sat, 02 Mar</t>
+  </si>
+  <si>
+    <t>30579286</t>
   </si>
   <si>
     <t>Sat, 09 Mar</t>
@@ -665,7 +839,7 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G37"/>
+  <dimension ref="A1:G66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -698,7 +872,7 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="n">
-        <v>44</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -721,807 +895,1474 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="n">
-        <v>46</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D3" t="s">
         <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" t="s">
         <v>15</v>
-      </c>
-      <c r="G3" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="n">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
         <v>17</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>18</v>
       </c>
-      <c r="D4" t="s">
-        <v>19</v>
-      </c>
       <c r="E4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" t="s">
         <v>20</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>21</v>
-      </c>
-      <c r="G4" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="n">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" t="s">
         <v>23</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" t="s">
         <v>24</v>
       </c>
-      <c r="D5" t="s">
+      <c r="G5" t="s">
         <v>25</v>
-      </c>
-      <c r="E5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="n">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="D6" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="E6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F6" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="G6" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="n">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D7" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="E7" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="F7" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="G7" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="n">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B8" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C8" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="D8" t="s">
-        <v>9</v>
+        <v>37</v>
       </c>
       <c r="E8" t="s">
-        <v>10</v>
+        <v>38</v>
       </c>
       <c r="F8" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="G8" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="n">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B9" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" t="s">
         <v>24</v>
       </c>
-      <c r="D9" t="s">
-        <v>38</v>
-      </c>
-      <c r="E9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" t="s">
-        <v>39</v>
-      </c>
       <c r="G9" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="n">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B10" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C10" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="D10" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="E10" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="F10" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="G10" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="n">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B11" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C11" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D11" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="E11" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="F11" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="G11" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="n">
+        <v>48</v>
+      </c>
+      <c r="B12" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" t="s">
+        <v>48</v>
+      </c>
+      <c r="G12" t="s">
         <v>49</v>
-      </c>
-      <c r="B12" t="s">
-        <v>43</v>
-      </c>
-      <c r="C12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D12" t="s">
-        <v>19</v>
-      </c>
-      <c r="E12" t="s">
-        <v>20</v>
-      </c>
-      <c r="F12" t="s">
-        <v>46</v>
-      </c>
-      <c r="G12" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="n">
+        <v>48</v>
+      </c>
+      <c r="B13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" t="s">
         <v>51</v>
       </c>
-      <c r="B13" t="s">
-        <v>48</v>
-      </c>
-      <c r="C13" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13" t="s">
-        <v>19</v>
-      </c>
-      <c r="E13" t="s">
-        <v>20</v>
-      </c>
-      <c r="F13" t="s">
-        <v>49</v>
-      </c>
       <c r="G13" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="n">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B14" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C14" t="s">
-        <v>24</v>
+        <v>54</v>
       </c>
       <c r="D14" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="E14" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="F14" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="G14" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="n">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B15" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="C15" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="D15" t="s">
-        <v>19</v>
+        <v>58</v>
       </c>
       <c r="E15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F15" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="G15" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="n">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B16" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C16" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="D16" t="s">
         <v>9</v>
       </c>
       <c r="E16" t="s">
-        <v>10</v>
+        <v>48</v>
       </c>
       <c r="F16" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="G16" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" t="n">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B17" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C17" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="D17" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="E17" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="F17" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="G17" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" t="n">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B18" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="C18" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="D18" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="E18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F18" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="G18" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" t="n">
-        <v>2</v>
+        <v>49</v>
       </c>
       <c r="B19" t="s">
         <v>64</v>
       </c>
       <c r="C19" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D19" t="s">
-        <v>38</v>
+        <v>67</v>
       </c>
       <c r="E19" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="F19" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="G19" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" t="n">
-        <v>2</v>
+        <v>49</v>
       </c>
       <c r="B20" t="s">
         <v>64</v>
       </c>
       <c r="C20" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D20" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="E20" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="F20" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="G20" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" t="n">
-        <v>2</v>
+        <v>50</v>
       </c>
       <c r="B21" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="C21" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D21" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="E21" t="s">
-        <v>10</v>
+        <v>38</v>
       </c>
       <c r="F21" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="G21" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" t="n">
-        <v>2</v>
+        <v>51</v>
       </c>
       <c r="B22" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="C22" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="D22" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="E22" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="F22" t="s">
-        <v>72</v>
+        <v>14</v>
       </c>
       <c r="G22" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" t="n">
-        <v>2</v>
+        <v>51</v>
       </c>
       <c r="B23" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="C23" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="D23" t="s">
-        <v>9</v>
+        <v>58</v>
       </c>
       <c r="E23" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="F23" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="G23" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" t="n">
-        <v>4</v>
+        <v>51</v>
       </c>
       <c r="B24" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C24" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D24" t="s">
-        <v>38</v>
+        <v>67</v>
       </c>
       <c r="E24" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="F24" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="G24" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" t="n">
-        <v>4</v>
+        <v>51</v>
       </c>
       <c r="B25" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C25" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="D25" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="E25" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="F25" t="s">
-        <v>60</v>
+        <v>82</v>
       </c>
       <c r="G25" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
     </row>
     <row r="26" spans="1:7">
       <c r="A26" t="n">
-        <v>4</v>
+        <v>52</v>
       </c>
       <c r="B26" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="C26" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D26" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="E26" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="F26" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="G26" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
     </row>
     <row r="27" spans="1:7">
       <c r="A27" t="n">
-        <v>4</v>
+        <v>52</v>
       </c>
       <c r="B27" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="C27" t="s">
-        <v>83</v>
+        <v>27</v>
       </c>
       <c r="D27" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="E27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F27" t="s">
-        <v>21</v>
+        <v>87</v>
       </c>
       <c r="G27" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
     </row>
     <row r="28" spans="1:7">
       <c r="A28" t="n">
-        <v>5</v>
+        <v>52</v>
       </c>
       <c r="B28" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C28" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="D28" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="E28" t="s">
-        <v>20</v>
+        <v>48</v>
       </c>
       <c r="F28" t="s">
-        <v>54</v>
+        <v>14</v>
       </c>
       <c r="G28" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="29" spans="1:7">
       <c r="A29" t="n">
-        <v>6</v>
+        <v>52</v>
       </c>
       <c r="B29" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C29" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="D29" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="E29" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="F29" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="G29" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="30" spans="1:7">
       <c r="A30" t="n">
-        <v>6</v>
+        <v>52</v>
       </c>
       <c r="B30" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C30" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="D30" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="E30" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="F30" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="G30" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row r="31" spans="1:7">
       <c r="A31" t="n">
-        <v>6</v>
+        <v>52</v>
       </c>
       <c r="B31" t="s">
         <v>92</v>
       </c>
       <c r="C31" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="D31" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="E31" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="F31" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="G31" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="32" spans="1:7">
       <c r="A32" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B32" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="C32" t="s">
-        <v>83</v>
+        <v>27</v>
       </c>
       <c r="D32" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="E32" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="F32" t="s">
-        <v>27</v>
+        <v>87</v>
       </c>
       <c r="G32" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="33" spans="1:7">
       <c r="A33" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B33" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="C33" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D33" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="E33" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="F33" t="s">
-        <v>49</v>
+        <v>100</v>
       </c>
       <c r="G33" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
     </row>
     <row r="34" spans="1:7">
       <c r="A34" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B34" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="C34" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D34" t="s">
-        <v>9</v>
+        <v>67</v>
       </c>
       <c r="E34" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="F34" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="G34" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
     </row>
     <row r="35" spans="1:7">
       <c r="A35" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B35" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C35" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D35" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="E35" t="s">
-        <v>10</v>
+        <v>48</v>
       </c>
       <c r="F35" t="s">
-        <v>101</v>
+        <v>85</v>
       </c>
       <c r="G35" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B36" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C36" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="D36" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="E36" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F36" t="s">
-        <v>46</v>
+        <v>11</v>
       </c>
       <c r="G36" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="37" spans="1:7">
       <c r="A37" t="n">
+        <v>2</v>
+      </c>
+      <c r="B37" t="s">
+        <v>99</v>
+      </c>
+      <c r="C37" t="s">
+        <v>50</v>
+      </c>
+      <c r="D37" t="s">
+        <v>18</v>
+      </c>
+      <c r="E37" t="s">
+        <v>19</v>
+      </c>
+      <c r="F37" t="s">
+        <v>106</v>
+      </c>
+      <c r="G37" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38" t="n">
+        <v>2</v>
+      </c>
+      <c r="B38" t="s">
+        <v>108</v>
+      </c>
+      <c r="C38" t="s">
+        <v>27</v>
+      </c>
+      <c r="D38" t="s">
+        <v>41</v>
+      </c>
+      <c r="E38" t="s">
+        <v>19</v>
+      </c>
+      <c r="F38" t="s">
+        <v>109</v>
+      </c>
+      <c r="G38" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39" t="n">
+        <v>2</v>
+      </c>
+      <c r="B39" t="s">
+        <v>108</v>
+      </c>
+      <c r="C39" t="s">
+        <v>31</v>
+      </c>
+      <c r="D39" t="s">
+        <v>32</v>
+      </c>
+      <c r="E39" t="s">
+        <v>33</v>
+      </c>
+      <c r="F39" t="s">
+        <v>85</v>
+      </c>
+      <c r="G39" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="A40" t="n">
+        <v>2</v>
+      </c>
+      <c r="B40" t="s">
+        <v>108</v>
+      </c>
+      <c r="C40" t="s">
+        <v>54</v>
+      </c>
+      <c r="D40" t="s">
+        <v>18</v>
+      </c>
+      <c r="E40" t="s">
+        <v>19</v>
+      </c>
+      <c r="F40" t="s">
+        <v>112</v>
+      </c>
+      <c r="G40" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41" t="n">
+        <v>3</v>
+      </c>
+      <c r="B41" t="s">
+        <v>114</v>
+      </c>
+      <c r="C41" t="s">
+        <v>27</v>
+      </c>
+      <c r="D41" t="s">
+        <v>67</v>
+      </c>
+      <c r="E41" t="s">
+        <v>19</v>
+      </c>
+      <c r="F41" t="s">
+        <v>100</v>
+      </c>
+      <c r="G41" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
+      <c r="A42" t="n">
+        <v>3</v>
+      </c>
+      <c r="B42" t="s">
+        <v>114</v>
+      </c>
+      <c r="C42" t="s">
+        <v>27</v>
+      </c>
+      <c r="D42" t="s">
+        <v>28</v>
+      </c>
+      <c r="E42" t="s">
+        <v>19</v>
+      </c>
+      <c r="F42" t="s">
+        <v>116</v>
+      </c>
+      <c r="G42" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="A43" t="n">
+        <v>3</v>
+      </c>
+      <c r="B43" t="s">
+        <v>114</v>
+      </c>
+      <c r="C43" t="s">
+        <v>27</v>
+      </c>
+      <c r="D43" t="s">
+        <v>9</v>
+      </c>
+      <c r="E43" t="s">
+        <v>19</v>
+      </c>
+      <c r="F43" t="s">
+        <v>85</v>
+      </c>
+      <c r="G43" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="A44" t="n">
+        <v>4</v>
+      </c>
+      <c r="B44" t="s">
+        <v>119</v>
+      </c>
+      <c r="C44" t="s">
+        <v>27</v>
+      </c>
+      <c r="D44" t="s">
+        <v>58</v>
+      </c>
+      <c r="E44" t="s">
+        <v>19</v>
+      </c>
+      <c r="F44" t="s">
+        <v>120</v>
+      </c>
+      <c r="G44" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
+      <c r="A45" t="n">
+        <v>4</v>
+      </c>
+      <c r="B45" t="s">
+        <v>119</v>
+      </c>
+      <c r="C45" t="s">
+        <v>27</v>
+      </c>
+      <c r="D45" t="s">
+        <v>9</v>
+      </c>
+      <c r="E45" t="s">
+        <v>48</v>
+      </c>
+      <c r="F45" t="s">
+        <v>19</v>
+      </c>
+      <c r="G45" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
+      <c r="A46" t="n">
+        <v>4</v>
+      </c>
+      <c r="B46" t="s">
+        <v>119</v>
+      </c>
+      <c r="C46" t="s">
+        <v>17</v>
+      </c>
+      <c r="D46" t="s">
+        <v>18</v>
+      </c>
+      <c r="E46" t="s">
+        <v>19</v>
+      </c>
+      <c r="F46" t="s">
+        <v>123</v>
+      </c>
+      <c r="G46" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
+      <c r="A47" t="n">
+        <v>4</v>
+      </c>
+      <c r="B47" t="s">
+        <v>125</v>
+      </c>
+      <c r="C47" t="s">
+        <v>27</v>
+      </c>
+      <c r="D47" t="s">
+        <v>41</v>
+      </c>
+      <c r="E47" t="s">
+        <v>19</v>
+      </c>
+      <c r="F47" t="s">
+        <v>126</v>
+      </c>
+      <c r="G47" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
+      <c r="A48" t="n">
+        <v>4</v>
+      </c>
+      <c r="B48" t="s">
+        <v>125</v>
+      </c>
+      <c r="C48" t="s">
+        <v>128</v>
+      </c>
+      <c r="D48" t="s">
+        <v>32</v>
+      </c>
+      <c r="E48" t="s">
+        <v>33</v>
+      </c>
+      <c r="F48" t="s">
+        <v>34</v>
+      </c>
+      <c r="G48" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
+      <c r="A49" t="n">
+        <v>5</v>
+      </c>
+      <c r="B49" t="s">
+        <v>130</v>
+      </c>
+      <c r="C49" t="s">
+        <v>27</v>
+      </c>
+      <c r="D49" t="s">
+        <v>37</v>
+      </c>
+      <c r="E49" t="s">
+        <v>38</v>
+      </c>
+      <c r="F49" t="s">
+        <v>85</v>
+      </c>
+      <c r="G49" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
+      <c r="A50" t="n">
+        <v>5</v>
+      </c>
+      <c r="B50" t="s">
+        <v>130</v>
+      </c>
+      <c r="C50" t="s">
+        <v>31</v>
+      </c>
+      <c r="D50" t="s">
+        <v>32</v>
+      </c>
+      <c r="E50" t="s">
+        <v>33</v>
+      </c>
+      <c r="F50" t="s">
+        <v>82</v>
+      </c>
+      <c r="G50" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
+      <c r="A51" t="n">
+        <v>6</v>
+      </c>
+      <c r="B51" t="s">
+        <v>133</v>
+      </c>
+      <c r="C51" t="s">
+        <v>27</v>
+      </c>
+      <c r="D51" t="s">
+        <v>58</v>
+      </c>
+      <c r="E51" t="s">
+        <v>19</v>
+      </c>
+      <c r="F51" t="s">
+        <v>102</v>
+      </c>
+      <c r="G51" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
+      <c r="A52" t="n">
+        <v>6</v>
+      </c>
+      <c r="B52" t="s">
+        <v>133</v>
+      </c>
+      <c r="C52" t="s">
+        <v>27</v>
+      </c>
+      <c r="D52" t="s">
+        <v>67</v>
+      </c>
+      <c r="E52" t="s">
+        <v>19</v>
+      </c>
+      <c r="F52" t="s">
+        <v>135</v>
+      </c>
+      <c r="G52" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7">
+      <c r="A53" t="n">
+        <v>6</v>
+      </c>
+      <c r="B53" t="s">
+        <v>133</v>
+      </c>
+      <c r="C53" t="s">
+        <v>27</v>
+      </c>
+      <c r="D53" t="s">
+        <v>28</v>
+      </c>
+      <c r="E53" t="s">
+        <v>19</v>
+      </c>
+      <c r="F53" t="s">
+        <v>137</v>
+      </c>
+      <c r="G53" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7">
+      <c r="A54" t="n">
+        <v>6</v>
+      </c>
+      <c r="B54" t="s">
+        <v>133</v>
+      </c>
+      <c r="C54" t="s">
+        <v>27</v>
+      </c>
+      <c r="D54" t="s">
+        <v>9</v>
+      </c>
+      <c r="E54" t="s">
+        <v>48</v>
+      </c>
+      <c r="F54" t="s">
+        <v>87</v>
+      </c>
+      <c r="G54" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7">
+      <c r="A55" t="n">
+        <v>6</v>
+      </c>
+      <c r="B55" t="s">
+        <v>133</v>
+      </c>
+      <c r="C55" t="s">
+        <v>27</v>
+      </c>
+      <c r="D55" t="s">
+        <v>9</v>
+      </c>
+      <c r="E55" t="s">
+        <v>19</v>
+      </c>
+      <c r="F55" t="s">
+        <v>46</v>
+      </c>
+      <c r="G55" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7">
+      <c r="A56" t="n">
+        <v>6</v>
+      </c>
+      <c r="B56" t="s">
+        <v>133</v>
+      </c>
+      <c r="C56" t="s">
+        <v>17</v>
+      </c>
+      <c r="D56" t="s">
+        <v>18</v>
+      </c>
+      <c r="E56" t="s">
+        <v>19</v>
+      </c>
+      <c r="F56" t="s">
+        <v>141</v>
+      </c>
+      <c r="G56" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7">
+      <c r="A57" t="n">
+        <v>6</v>
+      </c>
+      <c r="B57" t="s">
+        <v>143</v>
+      </c>
+      <c r="C57" t="s">
+        <v>27</v>
+      </c>
+      <c r="D57" t="s">
+        <v>41</v>
+      </c>
+      <c r="E57" t="s">
+        <v>19</v>
+      </c>
+      <c r="F57" t="s">
+        <v>144</v>
+      </c>
+      <c r="G57" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7">
+      <c r="A58" t="n">
+        <v>6</v>
+      </c>
+      <c r="B58" t="s">
+        <v>143</v>
+      </c>
+      <c r="C58" t="s">
+        <v>128</v>
+      </c>
+      <c r="D58" t="s">
+        <v>32</v>
+      </c>
+      <c r="E58" t="s">
+        <v>33</v>
+      </c>
+      <c r="F58" t="s">
+        <v>43</v>
+      </c>
+      <c r="G58" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7">
+      <c r="A59" t="n">
+        <v>7</v>
+      </c>
+      <c r="B59" t="s">
+        <v>147</v>
+      </c>
+      <c r="C59" t="s">
+        <v>27</v>
+      </c>
+      <c r="D59" t="s">
+        <v>37</v>
+      </c>
+      <c r="E59" t="s">
+        <v>38</v>
+      </c>
+      <c r="F59" t="s">
+        <v>148</v>
+      </c>
+      <c r="G59" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7">
+      <c r="A60" t="n">
+        <v>8</v>
+      </c>
+      <c r="B60" t="s">
+        <v>150</v>
+      </c>
+      <c r="C60" t="s">
+        <v>27</v>
+      </c>
+      <c r="D60" t="s">
+        <v>58</v>
+      </c>
+      <c r="E60" t="s">
+        <v>19</v>
+      </c>
+      <c r="F60" t="s">
+        <v>14</v>
+      </c>
+      <c r="G60" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7">
+      <c r="A61" t="n">
+        <v>8</v>
+      </c>
+      <c r="B61" t="s">
+        <v>150</v>
+      </c>
+      <c r="C61" t="s">
+        <v>27</v>
+      </c>
+      <c r="D61" t="s">
+        <v>37</v>
+      </c>
+      <c r="E61" t="s">
+        <v>38</v>
+      </c>
+      <c r="F61" t="s">
+        <v>152</v>
+      </c>
+      <c r="G61" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7">
+      <c r="A62" t="n">
+        <v>8</v>
+      </c>
+      <c r="B62" t="s">
+        <v>150</v>
+      </c>
+      <c r="C62" t="s">
+        <v>50</v>
+      </c>
+      <c r="D62" t="s">
+        <v>18</v>
+      </c>
+      <c r="E62" t="s">
+        <v>19</v>
+      </c>
+      <c r="F62" t="s">
+        <v>154</v>
+      </c>
+      <c r="G62" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7">
+      <c r="A63" t="n">
+        <v>8</v>
+      </c>
+      <c r="B63" t="s">
+        <v>156</v>
+      </c>
+      <c r="C63" t="s">
+        <v>27</v>
+      </c>
+      <c r="D63" t="s">
+        <v>41</v>
+      </c>
+      <c r="E63" t="s">
+        <v>19</v>
+      </c>
+      <c r="F63" t="s">
+        <v>157</v>
+      </c>
+      <c r="G63" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7">
+      <c r="A64" t="n">
+        <v>8</v>
+      </c>
+      <c r="B64" t="s">
+        <v>156</v>
+      </c>
+      <c r="C64" t="s">
+        <v>31</v>
+      </c>
+      <c r="D64" t="s">
+        <v>32</v>
+      </c>
+      <c r="E64" t="s">
+        <v>33</v>
+      </c>
+      <c r="F64" t="s">
+        <v>70</v>
+      </c>
+      <c r="G64" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7">
+      <c r="A65" t="n">
+        <v>9</v>
+      </c>
+      <c r="B65" t="s">
+        <v>160</v>
+      </c>
+      <c r="C65" t="s">
+        <v>27</v>
+      </c>
+      <c r="D65" t="s">
+        <v>28</v>
+      </c>
+      <c r="E65" t="s">
+        <v>19</v>
+      </c>
+      <c r="F65" t="s">
+        <v>87</v>
+      </c>
+      <c r="G65" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7">
+      <c r="A66" t="n">
         <v>10</v>
       </c>
-      <c r="B37" t="s">
-        <v>104</v>
-      </c>
-      <c r="C37" t="s">
-        <v>24</v>
-      </c>
-      <c r="D37" t="s">
-        <v>38</v>
-      </c>
-      <c r="E37" t="s">
-        <v>10</v>
-      </c>
-      <c r="F37" t="s">
-        <v>77</v>
-      </c>
-      <c r="G37" t="s">
-        <v>105</v>
+      <c r="B66" t="s">
+        <v>162</v>
+      </c>
+      <c r="C66" t="s">
+        <v>27</v>
+      </c>
+      <c r="D66" t="s">
+        <v>58</v>
+      </c>
+      <c r="E66" t="s">
+        <v>19</v>
+      </c>
+      <c r="F66" t="s">
+        <v>120</v>
+      </c>
+      <c r="G66" t="s">
+        <v>163</v>
       </c>
     </row>
   </sheetData>

</xml_diff>